<commit_message>
General updates and cleanups
General updates and cleanups
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -111,9 +111,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="208">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>

</xml_diff>

<commit_message>
Added JUNIT Tests classes
Added AgainstTimeTest class
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>שם מלא</t>
   </si>
@@ -111,9 +111,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="214">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -647,6 +653,34 @@
         <v>50.0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="209" t="n">
+        <v>43989.85160238426</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="209" t="n">
+        <v>43989.85160335648</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Computer pick delay removed
Downgraded computers turn pick delay
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="23">
   <si>
     <t>שם מלא</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>746389865</t>
+  </si>
+  <si>
+    <t>נגד הזמן</t>
+  </si>
+  <si>
+    <t>נגד המחשב</t>
   </si>
 </sst>
 </file>
@@ -120,9 +126,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -246,7 +255,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -804,6 +813,34 @@
         <v>15.0</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="55" t="n">
+        <v>43992.93096039352</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="n">
+        <v>115.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="55" t="n">
+        <v>43992.93201335648</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="n">
+        <v>70.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Game logic bug fix
Fixed an issue when pressing on the same card triggered a match
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="23">
   <si>
     <t>שם מלא</t>
   </si>
@@ -126,9 +126,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -255,7 +260,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -841,6 +846,48 @@
         <v>70.0</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="57" t="n">
+        <v>44014.56587277778</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="n">
+        <v>390.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="60" t="n">
+        <v>44014.58315222222</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="60" t="n">
+        <v>44014.583157002315</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>